<commit_message>
guardando cambios en el remoto.
</commit_message>
<xml_diff>
--- a/data_base1.xlsx
+++ b/data_base1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
   <si>
     <t>names</t>
   </si>
@@ -61,6 +61,15 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>B3</t>
   </si>
 </sst>
 </file>
@@ -378,15 +387,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -399,8 +408,17 @@
       <c r="D1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -413,8 +431,17 @@
       <c r="D2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>9</v>
+      </c>
+      <c r="F2">
+        <v>6</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -427,8 +454,17 @@
       <c r="D3">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+      <c r="G3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -441,8 +477,17 @@
       <c r="D4">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>6</v>
+      </c>
+      <c r="F4">
+        <v>7</v>
+      </c>
+      <c r="G4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -455,8 +500,17 @@
       <c r="D5">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>8</v>
+      </c>
+      <c r="G5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -469,8 +523,17 @@
       <c r="D6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <v>9</v>
+      </c>
+      <c r="G6">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -483,8 +546,17 @@
       <c r="D7">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -497,8 +569,17 @@
       <c r="D8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>7</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -511,8 +592,17 @@
       <c r="D9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>9</v>
+      </c>
+      <c r="F9">
+        <v>8</v>
+      </c>
+      <c r="G9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -525,8 +615,17 @@
       <c r="D10">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>9</v>
+      </c>
+      <c r="G10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -539,8 +638,17 @@
       <c r="D11">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>9</v>
+      </c>
+      <c r="G11">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -553,8 +661,17 @@
       <c r="D12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12">
+        <v>6</v>
+      </c>
+      <c r="G12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -567,8 +684,17 @@
       <c r="D13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <v>9</v>
+      </c>
+      <c r="F13">
+        <v>4</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -581,8 +707,17 @@
       <c r="D14">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>4</v>
+      </c>
+      <c r="G14">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -595,8 +730,17 @@
       <c r="D15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <v>7</v>
+      </c>
+      <c r="F15">
+        <v>6</v>
+      </c>
+      <c r="G15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -609,8 +753,17 @@
       <c r="D16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <v>4</v>
+      </c>
+      <c r="F16">
+        <v>79</v>
+      </c>
+      <c r="G16">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -623,8 +776,17 @@
       <c r="D17">
         <v>9</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>9</v>
+      </c>
+      <c r="G17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -637,8 +799,17 @@
       <c r="D18">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>3</v>
+      </c>
+      <c r="G18">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>1</v>
       </c>
@@ -651,8 +822,17 @@
       <c r="D19">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <v>5</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>2</v>
       </c>
@@ -665,8 +845,17 @@
       <c r="D20">
         <v>41</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <v>3</v>
+      </c>
+      <c r="F20">
+        <v>8</v>
+      </c>
+      <c r="G20">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -678,6 +867,15 @@
       </c>
       <c r="D21">
         <v>3</v>
+      </c>
+      <c r="E21">
+        <v>58</v>
+      </c>
+      <c r="F21">
+        <v>2</v>
+      </c>
+      <c r="G21">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>